<commit_message>
updates to EIS long list formatting
</commit_message>
<xml_diff>
--- a/output_templates/EIS Long List.xlsx
+++ b/output_templates/EIS Long List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\soundcast_dev2\output_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AB0108-188B-4F01-B2B0-87A9C9478F3B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A187C43C-A46F-4BC3-A173-55FB1DCB2C7F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{39483952-8B34-439F-B4F4-4B1AAC21A663}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <sheet name="2050 TOD" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -276,7 +275,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -307,6 +306,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -626,7 +635,7 @@
   <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,22 +803,22 @@
     </row>
     <row r="9" spans="1:11" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="18">
         <v>11.681913416</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="18">
         <v>10.484346499800001</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="18">
         <v>10.061315889299999</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="18">
         <v>10.060106218</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="18">
         <v>10.1979192295</v>
       </c>
       <c r="H9" s="11"/>
@@ -1006,22 +1015,22 @@
     </row>
     <row r="17" spans="1:11" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="18">
         <v>4.7283447439100001</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="18">
         <v>4.2778908694300002</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="18">
         <v>4.2205415628000003</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="18">
         <v>4.1420150659799999</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="18">
         <v>4.1710798167199998</v>
       </c>
       <c r="H17" s="11"/>
@@ -1419,22 +1428,22 @@
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="19">
         <v>16.209856395799999</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="19">
         <v>14.107084885900001</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="19">
         <v>13.624563414100001</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="19">
         <v>13.430516701</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="19">
         <v>13.357984992700001</v>
       </c>
       <c r="H33" s="5"/>
@@ -2237,22 +2246,22 @@
       </c>
     </row>
     <row r="66" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="20">
         <v>0.38834793188299999</v>
       </c>
-      <c r="D66" s="7">
+      <c r="D66" s="20">
         <v>0.36313459345499999</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E66" s="21">
         <v>0.346954818138</v>
       </c>
-      <c r="F66" s="7">
+      <c r="F66" s="20">
         <v>0.34523008243800002</v>
       </c>
-      <c r="G66" s="7">
+      <c r="G66" s="20">
         <v>0.34437096602900003</v>
       </c>
       <c r="H66" s="7"/>
@@ -2459,22 +2468,22 @@
       </c>
     </row>
     <row r="74" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="20">
         <v>0.70971976766599998</v>
       </c>
-      <c r="D74" s="7">
+      <c r="D74" s="20">
         <v>0.66395508894900002</v>
       </c>
-      <c r="E74" s="15">
+      <c r="E74" s="21">
         <v>0.63687835932299997</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F74" s="20">
         <v>0.63683469722200003</v>
       </c>
-      <c r="G74" s="7">
+      <c r="G74" s="20">
         <v>0.63479966655999998</v>
       </c>
       <c r="H74" s="7"/>
@@ -2679,22 +2688,22 @@
       </c>
     </row>
     <row r="82" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+      <c r="B82" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C82" s="4">
+      <c r="C82" s="22">
         <v>488657</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D82" s="22">
         <v>764389</v>
       </c>
-      <c r="E82" s="8">
+      <c r="E82" s="23">
         <v>960490</v>
       </c>
-      <c r="F82" s="4">
+      <c r="F82" s="22">
         <v>978359</v>
       </c>
-      <c r="G82" s="4">
+      <c r="G82" s="22">
         <v>988314</v>
       </c>
       <c r="H82" s="4"/>
@@ -2870,22 +2879,22 @@
       </c>
     </row>
     <row r="90" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
+      <c r="B90" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C90" s="13">
+      <c r="C90" s="24">
         <v>0.45599371425399998</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D90" s="25">
         <v>0.53521670146599998</v>
       </c>
-      <c r="E90" s="13">
+      <c r="E90" s="24">
         <v>0.55563783027699998</v>
       </c>
-      <c r="F90" s="6">
+      <c r="F90" s="25">
         <v>0.558063511475</v>
       </c>
-      <c r="G90" s="6">
+      <c r="G90" s="25">
         <v>0.54546598516099998</v>
       </c>
       <c r="H90" s="6"/>

</xml_diff>